<commit_message>
fix input 4-20mA measurement
</commit_message>
<xml_diff>
--- a/01.Docs/Format_message/Data fomat datalogger_ByTech,PLC comment.xlsx
+++ b/01.Docs/Format_message/Data fomat datalogger_ByTech,PLC comment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Project\BYT-Hawaco-GW\01.Docs\Format_message\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48383C7D-8634-4ED7-A8E9-6BA604DC31CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA3CDF6-DE0E-4883-ACFC-E98CBEE982FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhan cai dat-G1" sheetId="1" r:id="rId1"/>
@@ -1206,7 +1206,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
+    <comment ref="K5" authorId="1" shapeId="0" xr:uid="{61B2D46B-4CE2-4BC4-A606-A65D3882455D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tran Huy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+0 : disable
+1 : enable</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -1232,7 +1257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
+    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -1257,7 +1282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
+    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -1281,7 +1306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
+    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -1305,7 +1330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{CAC24948-B795-4C25-88C8-40B3695D59F8}">
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{CAC24948-B795-4C25-88C8-40B3695D59F8}">
       <text>
         <r>
           <rPr>
@@ -1330,7 +1355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -1355,7 +1380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
       <text>
         <r>
           <rPr>
@@ -1381,7 +1406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U5" authorId="1" shapeId="0" xr:uid="{22207E2C-3261-4BFE-B0B0-E361915A4F7F}">
+    <comment ref="V5" authorId="1" shapeId="0" xr:uid="{22207E2C-3261-4BFE-B0B0-E361915A4F7F}">
       <text>
         <r>
           <rPr>
@@ -1406,7 +1431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L26" authorId="0" shapeId="0" xr:uid="{8759B90B-4C0D-449D-B8A0-32FA78947DAD}">
+    <comment ref="M26" authorId="0" shapeId="0" xr:uid="{8759B90B-4C0D-449D-B8A0-32FA78947DAD}">
       <text>
         <r>
           <rPr>
@@ -1430,7 +1455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R26" authorId="0" shapeId="0" xr:uid="{C2B64400-E76B-47BF-87D8-D42164E438B6}">
+    <comment ref="S26" authorId="0" shapeId="0" xr:uid="{C2B64400-E76B-47BF-87D8-D42164E438B6}">
       <text>
         <r>
           <rPr>
@@ -1454,7 +1479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K28" authorId="0" shapeId="0" xr:uid="{654044C0-0271-4F77-92B2-1C509CBAF042}">
+    <comment ref="L28" authorId="0" shapeId="0" xr:uid="{654044C0-0271-4F77-92B2-1C509CBAF042}">
       <text>
         <r>
           <rPr>
@@ -1478,7 +1503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L28" authorId="0" shapeId="0" xr:uid="{4FD30D1A-DE4C-4837-B4CE-B3C7603361CC}">
+    <comment ref="M28" authorId="0" shapeId="0" xr:uid="{4FD30D1A-DE4C-4837-B4CE-B3C7603361CC}">
       <text>
         <r>
           <rPr>
@@ -1502,7 +1527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M28" authorId="0" shapeId="0" xr:uid="{F2E57F93-F1B9-4D65-B70A-F3C9D9A8BA86}">
+    <comment ref="N28" authorId="0" shapeId="0" xr:uid="{F2E57F93-F1B9-4D65-B70A-F3C9D9A8BA86}">
       <text>
         <r>
           <rPr>
@@ -1527,7 +1552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N28" authorId="0" shapeId="0" xr:uid="{171D00DF-113A-42E9-86F1-7DD6F1C90C53}">
+    <comment ref="O28" authorId="0" shapeId="0" xr:uid="{171D00DF-113A-42E9-86F1-7DD6F1C90C53}">
       <text>
         <r>
           <rPr>
@@ -1552,7 +1577,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R28" authorId="0" shapeId="0" xr:uid="{EBCAD827-397D-40AF-B6A3-29F5C895FA4A}">
+    <comment ref="S28" authorId="0" shapeId="0" xr:uid="{EBCAD827-397D-40AF-B6A3-29F5C895FA4A}">
       <text>
         <r>
           <rPr>
@@ -1576,7 +1601,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S28" authorId="0" shapeId="0" xr:uid="{C88AA738-1566-4013-B49E-CAA615FC91C9}">
+    <comment ref="T28" authorId="0" shapeId="0" xr:uid="{C88AA738-1566-4013-B49E-CAA615FC91C9}">
       <text>
         <r>
           <rPr>
@@ -1601,7 +1626,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T28" authorId="0" shapeId="0" xr:uid="{7A592936-7E64-4721-B2F3-DB16350E3B0F}">
+    <comment ref="U28" authorId="0" shapeId="0" xr:uid="{7A592936-7E64-4721-B2F3-DB16350E3B0F}">
       <text>
         <r>
           <rPr>
@@ -1626,7 +1651,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L31" authorId="0" shapeId="0" xr:uid="{33178A83-EEC4-4AEB-B8F7-B92996710537}">
+    <comment ref="M31" authorId="0" shapeId="0" xr:uid="{33178A83-EEC4-4AEB-B8F7-B92996710537}">
       <text>
         <r>
           <rPr>
@@ -1650,7 +1675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R31" authorId="0" shapeId="0" xr:uid="{143072B3-8E5B-4235-B356-21A8BB2F3EF3}">
+    <comment ref="S31" authorId="0" shapeId="0" xr:uid="{143072B3-8E5B-4235-B356-21A8BB2F3EF3}">
       <text>
         <r>
           <rPr>
@@ -1674,7 +1699,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K33" authorId="0" shapeId="0" xr:uid="{43885D7E-F129-44E5-BA3B-F066A76F57AB}">
+    <comment ref="L33" authorId="0" shapeId="0" xr:uid="{43885D7E-F129-44E5-BA3B-F066A76F57AB}">
       <text>
         <r>
           <rPr>
@@ -1698,7 +1723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L33" authorId="0" shapeId="0" xr:uid="{5E56498E-119C-4028-BE0D-F2DFD52D12E5}">
+    <comment ref="M33" authorId="0" shapeId="0" xr:uid="{5E56498E-119C-4028-BE0D-F2DFD52D12E5}">
       <text>
         <r>
           <rPr>
@@ -1722,7 +1747,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M33" authorId="0" shapeId="0" xr:uid="{8DD64732-9195-4661-8F61-8F855714143F}">
+    <comment ref="N33" authorId="0" shapeId="0" xr:uid="{8DD64732-9195-4661-8F61-8F855714143F}">
       <text>
         <r>
           <rPr>
@@ -1747,7 +1772,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N33" authorId="0" shapeId="0" xr:uid="{C7F37B02-2E7F-46F9-81A4-5815D11D9CE9}">
+    <comment ref="O33" authorId="0" shapeId="0" xr:uid="{C7F37B02-2E7F-46F9-81A4-5815D11D9CE9}">
       <text>
         <r>
           <rPr>
@@ -1771,7 +1796,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R33" authorId="0" shapeId="0" xr:uid="{42DC9993-AA2C-4137-86A2-F36AC6B9E8B2}">
+    <comment ref="S33" authorId="0" shapeId="0" xr:uid="{42DC9993-AA2C-4137-86A2-F36AC6B9E8B2}">
       <text>
         <r>
           <rPr>
@@ -1795,7 +1820,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S33" authorId="0" shapeId="0" xr:uid="{B97BB43D-07DC-41F3-A5C3-DAD74D3104E6}">
+    <comment ref="T33" authorId="0" shapeId="0" xr:uid="{B97BB43D-07DC-41F3-A5C3-DAD74D3104E6}">
       <text>
         <r>
           <rPr>
@@ -1820,7 +1845,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T33" authorId="0" shapeId="0" xr:uid="{B75F5E04-4E43-490E-BBE6-4AEE21D90AAB}">
+    <comment ref="U33" authorId="0" shapeId="0" xr:uid="{B75F5E04-4E43-490E-BBE6-4AEE21D90AAB}">
       <text>
         <r>
           <rPr>
@@ -2366,7 +2391,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="263">
   <si>
     <t>ID Datalogger</t>
   </si>
@@ -3169,6 +3194,12 @@
   </si>
   <si>
     <t>SIM IMEI</t>
+  </si>
+  <si>
+    <t>Ngõ vào tín hiệu 4-20mA</t>
+  </si>
+  <si>
+    <t>Input_J3_1 (J3_2, J3_3,J3_4)</t>
   </si>
 </sst>
 </file>
@@ -3481,6 +3512,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3499,10 +3534,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3981,7 +4012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="Q33" sqref="H26:Q33"/>
     </sheetView>
   </sheetViews>
@@ -4649,10 +4680,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:V39"/>
+  <dimension ref="A2:W39"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4663,19 +4694,19 @@
     <col min="4" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="36.7109375" customWidth="1"/>
-    <col min="10" max="10" width="42.140625" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" customWidth="1"/>
-    <col min="13" max="14" width="22.28515625" customWidth="1"/>
-    <col min="15" max="15" width="22.7109375" customWidth="1"/>
-    <col min="16" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" customWidth="1"/>
-    <col min="19" max="19" width="34.28515625" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" customWidth="1"/>
-    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="10" max="11" width="42.140625" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" customWidth="1"/>
+    <col min="14" max="15" width="22.28515625" customWidth="1"/>
+    <col min="16" max="16" width="22.7109375" customWidth="1"/>
+    <col min="17" max="18" width="15.7109375" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="34.28515625" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>59</v>
       </c>
@@ -4707,43 +4738,46 @@
         <v>163</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="N2" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="O2" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>182</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>228</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4775,51 +4809,54 @@
         <v>164</v>
       </c>
       <c r="K3" t="s">
+        <v>261</v>
+      </c>
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>12</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="N3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="Q3" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="R3" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>252</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>181</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>229</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M4" s="13"/>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
-      <c r="R4" s="8"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R4" s="13"/>
+      <c r="S4" s="8"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -4851,42 +4888,44 @@
         <v>1</v>
       </c>
       <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
         <v>0</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>1</v>
-      </c>
-      <c r="M5" s="12">
-        <v>123456</v>
       </c>
       <c r="N5" s="12">
         <v>123456</v>
       </c>
-      <c r="O5" s="13">
-        <v>1</v>
+      <c r="O5" s="12">
+        <v>123456</v>
       </c>
       <c r="P5" s="13">
         <v>1</v>
       </c>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="8">
+      <c r="Q5" s="13">
         <v>1</v>
       </c>
-      <c r="S5" t="s">
+      <c r="R5" s="13"/>
+      <c r="S5" s="8">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
         <v>183</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>184</v>
       </c>
-      <c r="U5" s="31" t="s">
+      <c r="V5" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>1231</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M8" s="14"/>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
@@ -4896,12 +4935,12 @@
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
       <c r="V8" s="14"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M9" s="14" t="s">
+      <c r="W8" s="14"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="N9" s="14"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
@@ -4910,12 +4949,12 @@
       <c r="T9" s="14"/>
       <c r="U9" s="14"/>
       <c r="V9" s="14"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M10" s="14" t="s">
+      <c r="W9" s="14"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="14"/>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
@@ -4924,9 +4963,9 @@
       <c r="T10" s="14"/>
       <c r="U10" s="14"/>
       <c r="V10" s="14"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M11" s="14"/>
+      <c r="W10" s="14"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
@@ -4936,12 +4975,12 @@
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
       <c r="V11" s="14"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M12" s="14" t="s">
+      <c r="W11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
@@ -4950,12 +4989,12 @@
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M13" s="14" t="s">
+      <c r="W12" s="14"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -4964,12 +5003,12 @@
       <c r="T13" s="14"/>
       <c r="U13" s="14"/>
       <c r="V13" s="14"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W13" s="14"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I14" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="M14" s="14"/>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
@@ -4979,15 +5018,15 @@
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
       <c r="V14" s="14"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W14" s="14"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I15" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="N15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -4996,105 +5035,105 @@
       <c r="T15" s="14"/>
       <c r="U15" s="14"/>
       <c r="V15" s="14"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W15" s="14"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I16" s="29" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I17" s="30" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I18" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I19" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I20" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="K22" t="s">
+    <row r="22" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I23" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I24" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I25" s="29" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
         <v>205</v>
       </c>
-      <c r="K26" s="34" t="s">
+      <c r="L26" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="L26" s="34" t="s">
+      <c r="M26" s="34" t="s">
         <v>236</v>
       </c>
-      <c r="M26" s="34" t="s">
+      <c r="N26" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="N26" s="34" t="s">
+      <c r="O26" s="34" t="s">
         <v>238</v>
       </c>
-      <c r="O26" s="34" t="s">
+      <c r="P26" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="P26" s="37" t="s">
+      <c r="Q26" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="Q26" s="37"/>
-      <c r="R26" s="34" t="s">
+      <c r="R26" s="37"/>
+      <c r="S26" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="S26" s="34" t="s">
+      <c r="T26" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="T26" s="34" t="s">
+      <c r="U26" s="34" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I27" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="K27" s="37"/>
       <c r="L27" s="37"/>
       <c r="M27" s="37"/>
       <c r="N27" s="37"/>
@@ -5104,38 +5143,38 @@
       <c r="R27" s="37"/>
       <c r="S27" s="37"/>
       <c r="T27" s="37"/>
-    </row>
-    <row r="28" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="U27" s="37"/>
+    </row>
+    <row r="28" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I28" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="K28" s="37">
+      <c r="L28" s="37">
         <v>1</v>
       </c>
-      <c r="L28" s="37">
+      <c r="M28" s="37">
         <v>30001</v>
       </c>
-      <c r="M28" s="37" t="s">
+      <c r="N28" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="N28" s="37" t="s">
+      <c r="O28" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="O28" s="37"/>
       <c r="P28" s="37"/>
       <c r="Q28" s="37"/>
-      <c r="R28" s="37">
+      <c r="R28" s="37"/>
+      <c r="S28" s="37">
         <v>30001</v>
       </c>
-      <c r="S28" s="37" t="s">
+      <c r="T28" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="T28" s="37" t="s">
+      <c r="U28" s="37" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="K29" s="37"/>
+    <row r="29" spans="9:21" x14ac:dyDescent="0.25">
       <c r="L29" s="37"/>
       <c r="M29" s="37"/>
       <c r="N29" s="37"/>
@@ -5145,9 +5184,9 @@
       <c r="R29" s="37"/>
       <c r="S29" s="37"/>
       <c r="T29" s="37"/>
-    </row>
-    <row r="30" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="K30" s="37"/>
+      <c r="U29" s="37"/>
+    </row>
+    <row r="30" spans="9:21" x14ac:dyDescent="0.25">
       <c r="L30" s="37"/>
       <c r="M30" s="37"/>
       <c r="N30" s="37"/>
@@ -5157,35 +5196,35 @@
       <c r="R30" s="37"/>
       <c r="S30" s="37"/>
       <c r="T30" s="37"/>
-    </row>
-    <row r="31" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="K31" s="34" t="s">
+      <c r="U30" s="37"/>
+    </row>
+    <row r="31" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="L31" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="L31" s="34" t="s">
+      <c r="M31" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="M31" s="34" t="s">
+      <c r="N31" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="N31" s="34" t="s">
+      <c r="O31" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="O31" s="34"/>
-      <c r="P31" s="37"/>
+      <c r="P31" s="34"/>
       <c r="Q31" s="37"/>
-      <c r="R31" s="34" t="s">
+      <c r="R31" s="37"/>
+      <c r="S31" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="S31" s="34" t="s">
+      <c r="T31" s="34" t="s">
         <v>247</v>
       </c>
-      <c r="T31" s="34" t="s">
+      <c r="U31" s="34" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="32" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="K32" s="37"/>
+    <row r="32" spans="9:21" x14ac:dyDescent="0.25">
       <c r="L32" s="37"/>
       <c r="M32" s="37"/>
       <c r="N32" s="37"/>
@@ -5195,41 +5234,42 @@
       <c r="R32" s="37"/>
       <c r="S32" s="37"/>
       <c r="T32" s="37"/>
-    </row>
-    <row r="33" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="K33" s="37">
+      <c r="U32" s="37"/>
+    </row>
+    <row r="33" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="L33" s="37">
         <v>2</v>
       </c>
-      <c r="L33" s="37">
+      <c r="M33" s="37">
         <v>40001</v>
       </c>
-      <c r="M33" s="37" t="s">
+      <c r="N33" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="N33" s="37" t="s">
+      <c r="O33" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="O33" s="37"/>
       <c r="P33" s="37"/>
       <c r="Q33" s="37"/>
-      <c r="R33" s="37">
+      <c r="R33" s="37"/>
+      <c r="S33" s="37">
         <v>40001</v>
       </c>
-      <c r="S33" s="37" t="s">
+      <c r="T33" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="T33" s="37" t="s">
+      <c r="U33" s="37" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
         <v>254</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U5" r:id="rId1" xr:uid="{43106A11-763C-4094-B5DE-9DD618B00409}"/>
+    <hyperlink ref="V5" r:id="rId1" xr:uid="{43106A11-763C-4094-B5DE-9DD618B00409}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -5241,8 +5281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:AD23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5261,7 +5301,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:30" s="34" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="34" t="s">
@@ -5318,13 +5358,13 @@
       <c r="S2" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="T2" s="49" t="s">
+      <c r="T2" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="49" t="s">
+      <c r="U2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="49" t="s">
+      <c r="V2" s="43" t="s">
         <v>13</v>
       </c>
       <c r="W2" s="34" t="s">
@@ -5428,7 +5468,7 @@
       <c r="Y3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="Z3" s="50" t="s">
+      <c r="Z3" s="44" t="s">
         <v>258</v>
       </c>
       <c r="AA3" s="15" t="s">
@@ -5455,8 +5495,8 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="50"/>
-      <c r="AA4" s="50"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
     </row>
     <row r="5" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -5534,8 +5574,8 @@
       <c r="Y5" s="8">
         <v>1</v>
       </c>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
+      <c r="Z5" s="44"/>
+      <c r="AA5" s="44"/>
       <c r="AB5" t="s">
         <v>183</v>
       </c>
@@ -5998,14 +6038,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
@@ -6020,16 +6060,16 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="47" t="s">
         <v>66</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -6046,10 +6086,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="45"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="18" t="s">
         <v>69</v>
       </c>
@@ -6534,7 +6574,7 @@
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
-      <c r="G36" s="43" t="s">
+      <c r="G36" s="45" t="s">
         <v>115</v>
       </c>
       <c r="H36" s="21" t="s">
@@ -6552,7 +6592,7 @@
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
-      <c r="G37" s="44"/>
+      <c r="G37" s="46"/>
       <c r="H37" s="22" t="s">
         <v>111</v>
       </c>

</xml_diff>